<commit_message>
Update of the dummy data.
</commit_message>
<xml_diff>
--- a/tests/test_utilities/patient_data_2020_07_obfuscated.xlsx
+++ b/tests/test_utilities/patient_data_2020_07_obfuscated.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/marekpolak/Projects/kidney-exchange/tests/test_utilities/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D6032A1-B099-FC4B-8167-A8C24C225567}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{04FAA39D-E1FA-F242-9288-4FBFCC065F7D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="76800" windowHeight="42740" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -88,9 +88,6 @@
     <t>P2</t>
   </si>
   <si>
-    <t>A2 A26 B27 B62 DR1 DR8</t>
-  </si>
-  <si>
     <t>A68 A34 Cw5 A69 B64 A33 B39 B65 A29 B8 B38 B54 DR53 DR7 DQ2 DQ7 DQ9 DR52 DQ4 DR12 DQ8 DR9 DR10</t>
   </si>
   <si>
@@ -106,6 +103,37 @@
     <t>A2 A11 B46 DR9</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="238"/>
+      </rPr>
+      <t>B60 B61 B48 B7 B81 B76 B49 B8 B50 B62 B39 B67 B72 B47 B41 B51 B27 B44 B18 B45 B78 B42 B64 B71 B38 B13 B55 B37 B73 B59 B53 B77 B56 B35 B75 B54 B52 B65 A32 B57 B82 B63 A1 B58 A66 A23 A25 Cw2 A24 A36 A80 Cw17 A29</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="238"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="238"/>
+      </rPr>
+      <t>DR13 DR16 DR14 DR15 DR17 DR8 DR12 DR11 DR52 DR18 DR10 DR103 DR4 DR1 DR51 DQ6</t>
+    </r>
+  </si>
+  <si>
     <t>0, B</t>
   </si>
   <si>
@@ -115,9 +143,6 @@
     <t>A1 A68 B8 B53 DR9 DR13 DR53 DR52 DQ9 DQ6</t>
   </si>
   <si>
-    <t>P4</t>
-  </si>
-  <si>
     <r>
       <rPr>
         <sz val="10"/>
@@ -226,18 +251,9 @@
     <t>Cw1 Cw12 Cw15</t>
   </si>
   <si>
-    <t>D7</t>
-  </si>
-  <si>
     <t>A2 A68 B65 B44 DR13 DR52 DQ7 DQ6</t>
   </si>
   <si>
-    <t>P7</t>
-  </si>
-  <si>
-    <t>A2 A68 B41 B65 DR11 DR13</t>
-  </si>
-  <si>
     <r>
       <rPr>
         <sz val="8"/>
@@ -311,6 +327,9 @@
     <t xml:space="preserve">A1 B7 B8 DR4 DR7 </t>
   </si>
   <si>
+    <t>A32 B44 B57 B18 B49 A3 B45 B51 B38 A23 B53 B58 B63 A25 B76 A74 B77 B37 B59 B13 B47 B52 B82 A24 B27 B54 B64 B72 A2 A31 B35 A33 B62 B78 B46 B50 A29 A68 A66 B71 A34 B75 B65 B56 A36 A69 A80 A11 A30 B67 B39 B55 DQ6 DQ5 DR17 DR13 DR18 DQ7 DQ4 DR52 DQ2 DR14 DR103 DR12 DR8 DR11 DR4 DP4 DR51 DR16 DP1 DP5 DP11 DP13 DP19 DP23 DR15 DP15 DR10</t>
+  </si>
+  <si>
     <t>D11</t>
   </si>
   <si>
@@ -323,6 +342,9 @@
     <t xml:space="preserve">A2 A26 B49 B51 DR13 </t>
   </si>
   <si>
+    <t>DQ9 DQ8 DP13 DR4 DQ4 DR51 DP14 DR7 DR13</t>
+  </si>
+  <si>
     <t>D12</t>
   </si>
   <si>
@@ -335,150 +357,87 @@
     <t>A1 A23 B8 B35 DR17 DR11 DR52 DQ2 DQ7 DP1 DP4</t>
   </si>
   <si>
-    <t>W-57D1</t>
-  </si>
-  <si>
     <t>A11 A31 B35 B51 Cw4 Cw15 DR14 DR15 DR52 DR51 DQ5 DQ6</t>
   </si>
   <si>
-    <t>W-57R</t>
-  </si>
-  <si>
     <t xml:space="preserve">A30 A31 B13 B51 DR7 DR15 </t>
   </si>
   <si>
     <t>A24 A23 A1 A36 A3 A11  B37 B76 A2 B57 A69 A68 A29 A80 B73 DQ7 DQ9 DQ8 DR12 DR8 DR13 DR14 DR17 DR11 DR18 DP28 DR52 B35 Cw4</t>
   </si>
   <si>
-    <t>W-59D1</t>
-  </si>
-  <si>
     <t>A1 A26 B8 B38 Cw7 Cw12 DR13 DR52 DQ6 DQ8</t>
   </si>
   <si>
-    <t>W-59R</t>
-  </si>
-  <si>
-    <t>A2 A68 B8 B35 DR1 DR7</t>
-  </si>
-  <si>
     <t>B76 DR4 DR8 DR11 DR13 DR14 DR15 DR16 DR17 DR18 DR52 DR53</t>
   </si>
   <si>
-    <t>W-60D2</t>
-  </si>
-  <si>
     <t>A3 A31 B7 B51 Cw7 Cw15 DR7 DR8 DR53 DQ9 DQ4</t>
   </si>
   <si>
-    <t>W-60R</t>
-  </si>
-  <si>
     <t xml:space="preserve">A2 B27 B38 DR15 DR13 </t>
   </si>
   <si>
     <t>A1 A11 A25 A26 A34 A43 A66 A32 B62 A68 B35 B49 B50 B51 B52 B56 B57 B63 B71 B72 B75 B76 B77 Cw9 Cw10 DQ2 DQ4 DQ7 DQ8 DQ9 DR7 DR9 DR10 DR53 DR14 DR4 B13 B78 B53</t>
   </si>
   <si>
-    <t>W-63D1</t>
-  </si>
-  <si>
-    <t>A1 A68 B8 B60 Cw10 Cw7 DR1 DR17 DR52 DQ5 DQ2</t>
-  </si>
-  <si>
-    <t>W-63R</t>
-  </si>
-  <si>
     <t>A2 A68 B35 B51 DR8 DR9</t>
   </si>
   <si>
     <t>A1 A3 A11 A23 A24 A26 A29 A36 A80 B13 B27 B41 B44 B45 B47 B49 B50 B60 B61 B76 DQ2</t>
   </si>
   <si>
-    <t>W-64D1</t>
-  </si>
-  <si>
     <t>A3 A31 B51 B57 Cw6 Cw14 DR4 DR13 DR52 DR53 DQ7 DQ8</t>
   </si>
   <si>
-    <t>W-64R</t>
-  </si>
-  <si>
     <t xml:space="preserve">A2 B65 B60 DR13 DR14 </t>
   </si>
   <si>
     <t>A23 A24 A25 A32 B18 B27 B35 B37 B38 B44 B47 B49 B51 B52 B53 B57 B58 B59 B63 B77 A66 B13 B78 A11 A26 A33 A34 A43 A68 A69 B62 B72 B75 B76 Cw4 Cw6 Cw7 Cw12 Cw17 DR1 DR51 DR9 DR10 DR53</t>
   </si>
   <si>
-    <t>W-65D1</t>
-  </si>
-  <si>
     <t>A1 A24 B8 B39 Cw7 DR1 DR7 DR53 DQ9 DQ5</t>
   </si>
   <si>
-    <t>W-65R</t>
-  </si>
-  <si>
     <t xml:space="preserve">A1 A3 B8 B13 DR1 DR16 </t>
   </si>
   <si>
     <t>A2 B77 Cw5 DQ2 DQ6 DQ7 DQ8 DQ9 DQ4</t>
   </si>
   <si>
-    <t>W-66D1</t>
-  </si>
-  <si>
     <t>A1 A3 B27 B39 Cw2 Cw12 DR11 DR16 DR52 DR51 DQ7 DQ5</t>
   </si>
   <si>
-    <t>W-66R</t>
-  </si>
-  <si>
     <t xml:space="preserve">A3 A24 B27 DR16 </t>
   </si>
   <si>
     <t>A2 A68 A69 B57 B73 B46 Cw10 A34 Cw8 B58 Cw7 Cw12 A31 Cw9 A25 A33 Cw14 A29 A11 Cw1 A66 A24 A26 Cw16 A30 A43 A36 Cw17 A74 A32 B55 B54 DQ6 DQ9 DQ7 DQ8 DQ4 DQ2 DR9 B45</t>
   </si>
   <si>
-    <t>W-68D1</t>
-  </si>
-  <si>
     <t>A1 A3 B8 B18 Cw7 DR17 DR12 DR52 DQ2 DQ7</t>
   </si>
   <si>
-    <t>W-68R</t>
-  </si>
-  <si>
     <t xml:space="preserve">A68 B71 DR17 DR15 </t>
   </si>
   <si>
     <t>A23 A24 A25 A32 B13 B27 B37 B38 B44 B47 B49 B51 B52 B53 B57 B58 B59 B63 B77 B35 B45 B50 B54 B55 B56 B62 B73 B76 B82 Cw1 Cw2 Cw4 Cw5 Cw6 Cw7 Cw8 Cw12 Cw14 Cw15 Cw16 Cw17 Cw18 A1 B39 B41 B48 B60 B61 B67 B75 B46</t>
   </si>
   <si>
-    <t>W-69D1</t>
-  </si>
-  <si>
     <t>A2 A68 B65 B27 Cw2 Cw8 DR1 DR13 DR52 DQ5 DQ7</t>
   </si>
   <si>
-    <t>W-69R</t>
-  </si>
-  <si>
     <t>A1 A2 B27 B37 DR1 DR10</t>
   </si>
   <si>
-    <t>W-71D1</t>
-  </si>
-  <si>
     <t>A1 A33 B65 B63 Cw7 Cw8 DR17 DR13 DR52 DQ2 DQ6</t>
   </si>
   <si>
-    <t>W-71R</t>
-  </si>
-  <si>
     <t xml:space="preserve">A1 A3 B7 B63 DR11 DR13 </t>
   </si>
   <si>
+    <t>A33 A31 B44 B8 B37 B82 A68 A69 A34 B18 B65 B64 B45 A66 A74 A29 A30 A25 DQ2 DQ5 DR52 DQ4</t>
+  </si>
+  <si>
     <t>D1001</t>
   </si>
   <si>
@@ -509,6 +468,9 @@
     <t>A2 B35 B51 DR4</t>
   </si>
   <si>
+    <t>A1 A3 A11 A23 A24 A25 A26 A29 A30 A32 A34 A36 A43 A66 A68 A80 B8 B45 B59 DQ6 DQ7 DR4 DR7 DR8 DR9 DR11 DR12 DR13 DR14 DR15 DR16 DR17 DR18 DR51 DR52</t>
+  </si>
+  <si>
     <t>D1003</t>
   </si>
   <si>
@@ -612,6 +574,98 @@
     <t>A33 A66 B41 B53 DR8 DR13</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="238"/>
+      </rPr>
+      <t xml:space="preserve">A1 A2 A3 A11 A24 A29 A30 A31 A32 A36 A43 A68 A69 A74 A80 B14 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="238"/>
+      </rPr>
+      <t>(B64, B65)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="238"/>
+      </rPr>
+      <t xml:space="preserve"> B15</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="238"/>
+      </rPr>
+      <t xml:space="preserve"> (B62, B63, B75. B76, B77)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="238"/>
+      </rPr>
+      <t xml:space="preserve"> B46 B49 B50 B56 B57 B58 B73 Cw1 Cw3 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="238"/>
+      </rPr>
+      <t>(Cw9, Cw10)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="238"/>
+      </rPr>
+      <t xml:space="preserve"> Cw5 Cw7 Cw8 Cw12 Cw14 Cw16 DQ2 DQ3 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="238"/>
+      </rPr>
+      <t>(DQ7, DQ8, DQ9)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="238"/>
+      </rPr>
+      <t xml:space="preserve"> DQ4 DQ5 DQ6 DR1 DR4 DR10 DR52</t>
+    </r>
+  </si>
+  <si>
     <t>D1027</t>
   </si>
   <si>
@@ -801,9 +855,6 @@
     <t>P1030</t>
   </si>
   <si>
-    <t>A1 A26 B27 B57 DR1 DR13</t>
-  </si>
-  <si>
     <r>
       <rPr>
         <sz val="8"/>
@@ -909,12 +960,39 @@
     </r>
   </si>
   <si>
-    <t>P1013</t>
-  </si>
-  <si>
     <t>A1 B51 DR11</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">A2 A3 A11 A24 A25 A26 A29 A30 A31 A33 A34 A43 A66 A68 A69 A74 B7 B27 B57 B58 B61 B81 DP1 DP3 DP5 DP9 DP11 DP13 DQ5 DR1 DR8 DR15 DR16 DR17 DR18 DQ1 DQ2 DQ3 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="238"/>
+      </rPr>
+      <t>(DQ7, DQ8, DQ9)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve"> DQ4 DQ6 DR4 DR7 DR9 DR10 DR11 DR12 DR13 DR14 DR51 DR52 DR53</t>
+    </r>
+  </si>
+  <si>
     <t>D1033</t>
   </si>
   <si>
@@ -927,6 +1005,9 @@
     <t>A2 A68 B41 B51 DR10 DR13</t>
   </si>
   <si>
+    <t xml:space="preserve">DR4 DR8 DR11 DR13 DR15 DR16 DR52 </t>
+  </si>
+  <si>
     <t>D1036</t>
   </si>
   <si>
@@ -961,9 +1042,6 @@
     </r>
   </si>
   <si>
-    <t>P1036</t>
-  </si>
-  <si>
     <r>
       <rPr>
         <sz val="10"/>
@@ -1062,144 +1140,74 @@
   <si>
     <r>
       <rPr>
-        <sz val="8"/>
+        <sz val="10"/>
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
         <charset val="238"/>
       </rPr>
-      <t xml:space="preserve">A3 A23 A24 A25 A26 A34 A66 B7 B27 B13 B38 B39 B40 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="238"/>
-      </rPr>
-      <t>(B60, B61)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
+      <t>A26 A30 B38 Cw12 DR4 DR11 DR53 DR52 DQ3</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="238"/>
+      </rPr>
+      <t xml:space="preserve"> (DQ7, DQ8, DQ9) </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
         <charset val="238"/>
       </rPr>
-      <t xml:space="preserve"> B42 B47 B48 B54 B57 B67 B73 B81 Cw1 DQ4 DQ5 DQ6 </t>
-    </r>
-  </si>
-  <si>
-    <t>D1040</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
+      <t>DP3 DP4</t>
+    </r>
+  </si>
+  <si>
+    <t>D1041</t>
+  </si>
+  <si>
+    <t>A2 A29 B7 B52 Cw12 Cw15 DR10 DR15 DR51 DQ5 DQ6 DP2 DP4</t>
+  </si>
+  <si>
+    <t>P1041</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="8"/>
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
         <charset val="238"/>
       </rPr>
-      <t>A26 A30 B38 Cw12 DR4 DR11 DR53 DR52 DQ3</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="238"/>
-      </rPr>
-      <t xml:space="preserve"> (DQ7, DQ8, DQ9) </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
+      <t xml:space="preserve">A2 A23 A24 A25 A32 A69 B7 B13 B27 B37 B38 B44 B47 B49 B51 B52 B53 B57 B58 B59 B60 B61 B63 B73 B77 B81 DR17 DR18 DR4 DR7 DR8 DR9 DR11 DR12 DR13 DR14 DR15 DR16 DR52 DR53 DR51 DQ2 DQ3 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="238"/>
+      </rPr>
+      <t>(DQ7, DQ8, DQ9)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
         <charset val="238"/>
       </rPr>
-      <t>DP3 DP4</t>
-    </r>
-  </si>
-  <si>
-    <t>P1040</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="238"/>
-      </rPr>
-      <t>A30 A31 B14</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="238"/>
-      </rPr>
-      <t xml:space="preserve"> (B64, B65)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="238"/>
-      </rPr>
-      <t xml:space="preserve"> B38 DR1 DR11</t>
-    </r>
-  </si>
-  <si>
-    <t>D1041</t>
-  </si>
-  <si>
-    <t>A2 A29 B7 B52 Cw12 Cw15 DR10 DR15 DR51 DQ5 DQ6 DP2 DP4</t>
-  </si>
-  <si>
-    <t>P1041</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="238"/>
-      </rPr>
-      <t xml:space="preserve">A11 A68 B35 B14 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="238"/>
-      </rPr>
-      <t>(B64, B65)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="238"/>
-      </rPr>
-      <t xml:space="preserve"> DR1</t>
+      <t xml:space="preserve"> DP2 DP3 DP4 DP6 DP9 DP10 DP28 DP14 DP17 DP18 DP20</t>
     </r>
   </si>
   <si>
@@ -1379,66 +1387,232 @@
     <t>U Izraelcu jenom ty prirozene akceptovatelne - tedy ne AB0i protokol</t>
   </si>
   <si>
-    <t xml:space="preserve"> A34 A36 A43 A66 A68 A80 B8 B45 B59 DQ6 DQ7 DR4 DR7 DR8 DR9 DR11 DR12 DR13 DR14 DR15 DR16 DR17 DR18 DR51 DR52</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve"> A30 A31 A33 A34 A43 A66 A68 A69 A74 B7 B27 B57 B58 B61 B81 DP1 DP3 DP5 DP9 DP11 DP13 DQ5 DR1 DR8 DR15 DR16 DR17 DR18 DQ1 DQ2 DQ3 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="238"/>
-      </rPr>
-      <t>(DQ7, DQ8, DQ9)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve"> DQ4 DQ6 DR4 DR7 DR9 DR10 DR11 DR12 DR13 DR14 DR51 DR52 DR53</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">A2 A3 A11 A24 A25 A26 A29 DR4 DR8 DR11 DR13 DR15 DR16 DR52 </t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve"> DR17 DR18 DR4 DR7 DR8 DR9 DR11 DR12 DR13 DR14 DR15 DR16 DR52 DR53 DR51 DQ2 DQ3 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="238"/>
-      </rPr>
-      <t>(DQ7, DQ8, DQ9)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
+    <t>D68</t>
+  </si>
+  <si>
+    <t>D70</t>
+  </si>
+  <si>
+    <t>D66</t>
+  </si>
+  <si>
+    <t>D65</t>
+  </si>
+  <si>
+    <t>D69</t>
+  </si>
+  <si>
+    <t>D60</t>
+  </si>
+  <si>
+    <t>D63</t>
+  </si>
+  <si>
+    <t>D64</t>
+  </si>
+  <si>
+    <t>D59</t>
+  </si>
+  <si>
+    <t>D40</t>
+  </si>
+  <si>
+    <t>D57</t>
+  </si>
+  <si>
+    <t>P68</t>
+  </si>
+  <si>
+    <t>P70</t>
+  </si>
+  <si>
+    <t>P1038</t>
+  </si>
+  <si>
+    <t>P1037</t>
+  </si>
+  <si>
+    <t>P66</t>
+  </si>
+  <si>
+    <t>P65</t>
+  </si>
+  <si>
+    <t>P69</t>
+  </si>
+  <si>
+    <t>P60</t>
+  </si>
+  <si>
+    <t>P63</t>
+  </si>
+  <si>
+    <t>P64</t>
+  </si>
+  <si>
+    <t>P12</t>
+  </si>
+  <si>
+    <t>P13</t>
+  </si>
+  <si>
+    <t>P59</t>
+  </si>
+  <si>
+    <t>P40</t>
+  </si>
+  <si>
+    <t>P57</t>
+  </si>
+  <si>
+    <t>A2 B8 B35 DR1 DR7</t>
+  </si>
+  <si>
+    <t>A1 A68 B8 B51 Cw10 Cw7 DR1 DR17 DR52 DQ5 DQ2</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve"> A25 A26 A32 A33 A34 A36 A43 A66 A68 A69 A74 B7 B8 B13 B27 B35 B60 B61 B40 B41 B42 B46 B47 B48 B51 B53 B55 B73 B78 B81 Cw1 Cw2 Cw3 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="238"/>
+      </rPr>
+      <t>(Cw9, Cw10)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="238"/>
+      </rPr>
+      <t xml:space="preserve"> Cw4 Cw5 Cw8 Cw12 Cw14 Cw15 Cw16 Cw18 DP1 DP2 DP4 DP5 DP6 DP9 DP11 DP13 DP14 DP15 DP17 DP18 DP19 DP28 DQ1 DQ2 DQ3</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="238"/>
+      </rPr>
+      <t xml:space="preserve"> (DQ7, DQ8,DQ9)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="238"/>
+      </rPr>
+      <t xml:space="preserve"> DQ4 DQ5 DQ6 DR1 DR3 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="238"/>
+      </rPr>
+      <t>(DR17, DR18</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="238"/>
+      </rPr>
+      <t xml:space="preserve">) DR4 DR8 DR11 DR12 DR13 DR14 DR15 DR16 DR51 DR5 </t>
+    </r>
+  </si>
+  <si>
+    <t>A1 A26 B27 B38 DR1 DR13</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">A11 A29 B35 B14 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="238"/>
+      </rPr>
+      <t>(B64, B65)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
         <charset val="238"/>
       </rPr>
-      <t xml:space="preserve"> DP2 DP3 DP4 DP6 DP9 DP10 DP28 DP14 DP17 DP18 DP20</t>
-    </r>
-  </si>
-  <si>
-    <t>A2 A23 A24 A25 A32 A69 B7 B13 B27 B37 B38 B44 B47 B49 B51 B52 B53 B57 B58 B59 B60 B61 B63 B73 B77 B81 DQ9 DQ8 DP13 DR4 DQ4 DR51 DP14 DR7 DR13</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">A80 A36 A74 A31 A68 B55 A33 A30 B63 A1 A69 A29 B67 Cw9 B54 B78 Cw10 B50 B42 B49 B46 B45 B76 B56 B58 B44 B35 B57 B59 B73 B62 Cw8 Cw1 B18 B13 B53 B72 B75 B71 B27 B82 B64 A24 B51 A2 B77 B52 B47 B37 Cw14 B65 B39 </t>
+      <t xml:space="preserve"> DR1</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>A26 A31 B14</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="238"/>
+      </rPr>
+      <t xml:space="preserve"> (B64, B65)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="238"/>
+      </rPr>
+      <t xml:space="preserve"> B38 DR1 DR11</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">A3 A23 A24 A26 A34 A66 B7 B27 B13 B38 B39 B40 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="238"/>
+      </rPr>
+      <t>(B60, B61)</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="8"/>
+        <color rgb="FF000000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+        <charset val="238"/>
+      </rPr>
+      <t xml:space="preserve"> B42 B47 B48 B54 B57 B67 B73 B81 Cw1 DQ4 DQ5 DQ6 </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">A3 A26 A66 A34 A43 A11 A32 A80 A36 A74 A31 A68 B55 A33 A30 B63 A1 A69 A29 B67 Cw9 B54 B78 Cw10 B50 B42 B49 B46 B44 B35 B57 B59 B73 B62 Cw8 Cw1 B18 B13 B53 B72 B75 B71 B27 B82 B64 A24 B51 A2 B77 B52 B47 B37 Cw14 B65 B39 </t>
     </r>
     <r>
       <rPr>
@@ -1451,181 +1625,13 @@
     </r>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">A1 A2 A3 A11 A24 A29 A30 A31 A32 A36 A43 A68 A69 A74 A80 B14 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="238"/>
-      </rPr>
-      <t>(B64, B65)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="238"/>
-      </rPr>
-      <t xml:space="preserve"> B15</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="238"/>
-      </rPr>
-      <t xml:space="preserve"> (B62, B63, B75. B76, B77)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="238"/>
-      </rPr>
-      <t xml:space="preserve"> B46 B49 B50 B56 B57 B58 B73 Cw1 Cw3 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="238"/>
-      </rPr>
-      <t>(Cw9, Cw10)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="238"/>
-      </rPr>
-      <t xml:space="preserve"> Cw5 Cw7 Cw8 Cw12 Cw14 Cw16 DQ2 DQ3 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="238"/>
-      </rPr>
-      <t>(DQ7, DQ8, DQ9)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="238"/>
-      </rPr>
-      <t xml:space="preserve"> DQ4 DQ5 DQ6 DR1 DR4 DR10 DR52</t>
-    </r>
-  </si>
-  <si>
-    <t>A32 B44 B57 B18 B49 A3 B45 B51 B38 A23 B53 B58 B63 B76 A74 B77 B37 B59 B13 B47 B52 B82 A24 B27 B54 B64 B72 A2 A31 B35 A33 B62 B78 B46 B50 A29 A68 A66 B71 A34 B75 B65 B56 A36 A69 A80 A11 A30 B67 B39 B55 DQ6 DQ5 DR17 DR13 DR18 DQ7 DQ4 DR52 DQ2 DR14 DR103 DR12 DR8 DR11 DR4 DP4 DR51 DR16 DP1 DP5 DP11 DP13 DP19 DP23 DR15 DP15 DR10</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">A1 A3 A11 A23 A24 A26 A29 A30 A32 A34 A36 A43 A66 A68 A69 A74 B7 B8 B13 B27 B35 B60 B61 B40 B41 B42 B46 B47 B48 B51 B53 B55 B73 B78 B81 Cw1 Cw2 Cw3 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="238"/>
-      </rPr>
-      <t>(Cw9, Cw10)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="238"/>
-      </rPr>
-      <t xml:space="preserve"> Cw4 Cw5 Cw8 Cw12 Cw14 Cw15 Cw16 Cw18 DP1 DP2 DP4 DP5 DP6 DP9 DP11 DP13 DP14 DP15 DP17 DP18 DP19 DP28 DQ1 DQ2 DQ3</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="238"/>
-      </rPr>
-      <t xml:space="preserve"> (DQ7, DQ8,DQ9)</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="238"/>
-      </rPr>
-      <t xml:space="preserve"> DQ4 DQ5 DQ6 DR1 DR3 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="238"/>
-      </rPr>
-      <t>(DR17, DR18</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="238"/>
-      </rPr>
-      <t xml:space="preserve">) DR4 DR8 DR11 DR12 DR13 DR14 DR15 DR16 DR51 DR5 </t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve"> B48 B7 B81 B76 B49 B8 B50 B62 B39 B67 B72 B47 B41 B51 B27 B44 B18 B45 B78 B42 B64 B71 B38 B13 B55 B37 B73 B59 B53 B77 B56 B35 B75 B54 B52 B65 A32 B57 B82 B63 A1 B58 A66 A23 Cw2 A24 A36 A80 Cw17 A29</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="238"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="8"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="238"/>
-      </rPr>
-      <t>DR13 DR16 DR14 DR15 DR17 DR8 DR12 DR11 DR52 DR18 DR10 DR103 DR4 DR1 DR51 DQ6</t>
-    </r>
-  </si>
-  <si>
-    <t>A1 A11 A23 A24 A26 A32 A33 A31 B44 B8 B37 B82 A68 A69 A34 B18 B65 B64 B45 A66 A74 A29 A30 A25 DQ2 DQ5 DR52 DQ4</t>
+    <t>A2 A26 B35 B62 DR1 DR8</t>
+  </si>
+  <si>
+    <t>D71</t>
+  </si>
+  <si>
+    <t>A2 A3 B41 B65 DR11 DR13</t>
   </si>
 </sst>
 </file>
@@ -2393,8 +2399,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A2:I40"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="114" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H27" sqref="H27"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.5" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -2439,7 +2445,7 @@
     </row>
     <row r="3" spans="1:9" ht="28" x14ac:dyDescent="0.2">
       <c r="A3" s="8" t="s">
-        <v>9</v>
+        <v>99</v>
       </c>
       <c r="B3" s="9" t="s">
         <v>10</v>
@@ -2448,7 +2454,7 @@
         <v>11</v>
       </c>
       <c r="D3" s="11" t="s">
-        <v>19</v>
+        <v>101</v>
       </c>
       <c r="E3" s="9" t="s">
         <v>13</v>
@@ -2466,7 +2472,7 @@
     </row>
     <row r="4" spans="1:9" ht="28" x14ac:dyDescent="0.2">
       <c r="A4" s="15" t="s">
-        <v>17</v>
+        <v>182</v>
       </c>
       <c r="B4" s="16" t="s">
         <v>10</v>
@@ -2475,44 +2481,44 @@
         <v>18</v>
       </c>
       <c r="D4" s="18" t="s">
-        <v>12</v>
+        <v>193</v>
       </c>
       <c r="E4" s="16" t="s">
         <v>13</v>
       </c>
       <c r="F4" s="17" t="s">
-        <v>20</v>
+        <v>216</v>
       </c>
       <c r="G4" s="12"/>
       <c r="H4" s="19" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I4" s="14" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:9" ht="173" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:9" ht="48" x14ac:dyDescent="0.2">
       <c r="A5" s="8" t="s">
-        <v>22</v>
+        <v>183</v>
       </c>
       <c r="B5" s="16" t="s">
         <v>13</v>
       </c>
       <c r="C5" s="17" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="D5" s="11" t="s">
-        <v>155</v>
+        <v>194</v>
       </c>
       <c r="E5" s="16" t="s">
         <v>13</v>
       </c>
       <c r="F5" s="17" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="G5" s="12"/>
       <c r="H5" s="19" t="s">
-        <v>217</v>
+        <v>25</v>
       </c>
       <c r="I5" s="14" t="s">
         <v>26</v>
@@ -2520,7 +2526,7 @@
     </row>
     <row r="6" spans="1:9" ht="60" x14ac:dyDescent="0.2">
       <c r="A6" s="15" t="s">
-        <v>27</v>
+        <v>151</v>
       </c>
       <c r="B6" s="16">
         <v>0</v>
@@ -2529,44 +2535,44 @@
         <v>28</v>
       </c>
       <c r="D6" s="18" t="s">
-        <v>127</v>
+        <v>195</v>
       </c>
       <c r="E6" s="16" t="s">
         <v>10</v>
       </c>
       <c r="F6" s="17" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="G6" s="12"/>
       <c r="H6" s="19" t="s">
-        <v>213</v>
+        <v>215</v>
       </c>
       <c r="I6" s="14" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="28" x14ac:dyDescent="0.2">
       <c r="A7" s="8" t="s">
-        <v>32</v>
+        <v>123</v>
       </c>
       <c r="B7" s="16" t="s">
         <v>10</v>
       </c>
       <c r="C7" s="16" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D7" s="11" t="s">
-        <v>151</v>
+        <v>125</v>
       </c>
       <c r="E7" s="16">
         <v>0</v>
       </c>
       <c r="F7" s="16" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="G7" s="20"/>
       <c r="H7" s="19" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I7" s="21">
         <v>0</v>
@@ -2574,80 +2580,80 @@
     </row>
     <row r="8" spans="1:9" ht="28" x14ac:dyDescent="0.2">
       <c r="A8" s="15" t="s">
-        <v>37</v>
+        <v>131</v>
       </c>
       <c r="B8" s="16" t="s">
         <v>10</v>
       </c>
       <c r="C8" s="17" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D8" s="18" t="s">
-        <v>173</v>
+        <v>133</v>
       </c>
       <c r="E8" s="16" t="s">
         <v>10</v>
       </c>
       <c r="F8" s="22" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="G8" s="23"/>
       <c r="H8" s="19" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I8" s="14" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="24" x14ac:dyDescent="0.2">
       <c r="A9" s="8" t="s">
-        <v>42</v>
+        <v>149</v>
       </c>
       <c r="B9" s="16" t="s">
         <v>10</v>
       </c>
       <c r="C9" s="17" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D9" s="11" t="s">
-        <v>106</v>
+        <v>196</v>
       </c>
       <c r="E9" s="16" t="s">
         <v>10</v>
       </c>
       <c r="F9" s="22" t="s">
-        <v>45</v>
+        <v>218</v>
       </c>
       <c r="G9" s="12"/>
       <c r="H9" s="19" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="I9" s="14" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="28" x14ac:dyDescent="0.2">
       <c r="A10" s="15" t="s">
-        <v>47</v>
+        <v>184</v>
       </c>
       <c r="B10" s="9" t="s">
         <v>13</v>
       </c>
       <c r="C10" s="16" t="s">
-        <v>48</v>
+        <v>44</v>
       </c>
       <c r="D10" s="18" t="s">
-        <v>136</v>
+        <v>197</v>
       </c>
       <c r="E10" s="9">
         <v>0</v>
       </c>
       <c r="F10" s="16" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="G10" s="12"/>
       <c r="H10" s="19" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="I10" s="14" t="s">
         <v>16</v>
@@ -2655,26 +2661,26 @@
     </row>
     <row r="11" spans="1:9" ht="28" x14ac:dyDescent="0.2">
       <c r="A11" s="8" t="s">
-        <v>52</v>
+        <v>94</v>
       </c>
       <c r="B11" s="9" t="s">
         <v>10</v>
       </c>
       <c r="C11" s="16" t="s">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="D11" s="11" t="s">
-        <v>164</v>
+        <v>96</v>
       </c>
       <c r="E11" s="9">
         <v>0</v>
       </c>
       <c r="F11" s="16" t="s">
-        <v>55</v>
+        <v>51</v>
       </c>
       <c r="G11" s="12"/>
       <c r="H11" s="19" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="I11" s="14" t="s">
         <v>16</v>
@@ -2682,26 +2688,26 @@
     </row>
     <row r="12" spans="1:9" ht="60" x14ac:dyDescent="0.2">
       <c r="A12" s="15" t="s">
-        <v>56</v>
+        <v>113</v>
       </c>
       <c r="B12" s="9" t="s">
         <v>10</v>
       </c>
       <c r="C12" s="17" t="s">
-        <v>57</v>
+        <v>53</v>
       </c>
       <c r="D12" s="18" t="s">
-        <v>86</v>
+        <v>115</v>
       </c>
       <c r="E12" s="9" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="F12" s="22" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="G12" s="12"/>
       <c r="H12" s="19" t="s">
-        <v>215</v>
+        <v>57</v>
       </c>
       <c r="I12" s="14" t="s">
         <v>26</v>
@@ -2709,26 +2715,26 @@
     </row>
     <row r="13" spans="1:9" ht="28" x14ac:dyDescent="0.2">
       <c r="A13" s="8" t="s">
-        <v>61</v>
+        <v>185</v>
       </c>
       <c r="B13" s="9" t="s">
         <v>13</v>
       </c>
       <c r="C13" s="17" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="D13" s="11" t="s">
-        <v>123</v>
+        <v>198</v>
       </c>
       <c r="E13" s="9" t="s">
         <v>13</v>
       </c>
       <c r="F13" s="22" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="G13" s="12"/>
       <c r="H13" s="19" t="s">
-        <v>212</v>
+        <v>62</v>
       </c>
       <c r="I13" s="14" t="s">
         <v>16</v>
@@ -2736,13 +2742,13 @@
     </row>
     <row r="14" spans="1:9" ht="28" x14ac:dyDescent="0.2">
       <c r="A14" s="15" t="s">
-        <v>65</v>
+        <v>127</v>
       </c>
       <c r="B14" s="16" t="s">
         <v>10</v>
       </c>
       <c r="C14" s="17" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D14" s="24"/>
       <c r="E14" s="16"/>
@@ -2753,13 +2759,13 @@
     </row>
     <row r="15" spans="1:9" ht="28" x14ac:dyDescent="0.2">
       <c r="A15" s="8" t="s">
-        <v>67</v>
+        <v>136</v>
       </c>
       <c r="B15" s="16" t="s">
         <v>13</v>
       </c>
       <c r="C15" s="22" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D15" s="24"/>
       <c r="E15" s="16"/>
@@ -2770,26 +2776,26 @@
     </row>
     <row r="16" spans="1:9" ht="28" x14ac:dyDescent="0.2">
       <c r="A16" s="25" t="s">
-        <v>69</v>
+        <v>145</v>
       </c>
       <c r="B16" s="16" t="s">
         <v>13</v>
       </c>
       <c r="C16" s="26" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="D16" s="24" t="s">
-        <v>132</v>
+        <v>147</v>
       </c>
       <c r="E16" s="16">
         <v>0</v>
       </c>
       <c r="F16" s="27" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="G16" s="12"/>
       <c r="H16" s="19" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="I16" s="14" t="s">
         <v>16</v>
@@ -2797,26 +2803,26 @@
     </row>
     <row r="17" spans="1:9" ht="28" x14ac:dyDescent="0.2">
       <c r="A17" s="25" t="s">
-        <v>74</v>
+        <v>140</v>
       </c>
       <c r="B17" s="16" t="s">
         <v>10</v>
       </c>
       <c r="C17" s="22" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="D17" s="11" t="s">
-        <v>76</v>
+        <v>142</v>
       </c>
       <c r="E17" s="22" t="s">
         <v>10</v>
       </c>
       <c r="F17" s="22" t="s">
-        <v>77</v>
+        <v>208</v>
       </c>
       <c r="G17" s="12"/>
       <c r="H17" s="19" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="I17" s="14" t="s">
         <v>16</v>
@@ -2824,26 +2830,26 @@
     </row>
     <row r="18" spans="1:9" ht="36" x14ac:dyDescent="0.2">
       <c r="A18" s="28" t="s">
-        <v>79</v>
+        <v>186</v>
       </c>
       <c r="B18" s="29">
         <v>0</v>
       </c>
       <c r="C18" s="26" t="s">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="D18" s="30" t="s">
-        <v>81</v>
+        <v>199</v>
       </c>
       <c r="E18" s="31" t="s">
         <v>13</v>
       </c>
       <c r="F18" s="26" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="G18" s="32"/>
       <c r="H18" s="33" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="I18" s="14" t="s">
         <v>16</v>
@@ -2851,26 +2857,26 @@
     </row>
     <row r="19" spans="1:9" ht="28" x14ac:dyDescent="0.2">
       <c r="A19" s="34" t="s">
-        <v>84</v>
+        <v>103</v>
       </c>
       <c r="B19" s="22">
         <v>0</v>
       </c>
       <c r="C19" s="22" t="s">
-        <v>85</v>
+        <v>209</v>
       </c>
       <c r="D19" s="35" t="s">
-        <v>58</v>
+        <v>105</v>
       </c>
       <c r="E19" s="36">
         <v>0</v>
       </c>
       <c r="F19" s="22" t="s">
-        <v>87</v>
+        <v>75</v>
       </c>
       <c r="G19" s="32"/>
       <c r="H19" s="19" t="s">
-        <v>88</v>
+        <v>76</v>
       </c>
       <c r="I19" s="14" t="s">
         <v>16</v>
@@ -2878,26 +2884,26 @@
     </row>
     <row r="20" spans="1:9" ht="36" x14ac:dyDescent="0.2">
       <c r="A20" s="34" t="s">
-        <v>89</v>
+        <v>108</v>
       </c>
       <c r="B20" s="36">
         <v>0</v>
       </c>
       <c r="C20" s="22" t="s">
-        <v>90</v>
+        <v>77</v>
       </c>
       <c r="D20" s="35" t="s">
-        <v>169</v>
+        <v>110</v>
       </c>
       <c r="E20" s="36" t="s">
         <v>10</v>
       </c>
       <c r="F20" s="22" t="s">
-        <v>92</v>
+        <v>78</v>
       </c>
       <c r="G20" s="32"/>
       <c r="H20" s="19" t="s">
-        <v>93</v>
+        <v>79</v>
       </c>
       <c r="I20" s="14" t="s">
         <v>16</v>
@@ -2905,26 +2911,26 @@
     </row>
     <row r="21" spans="1:9" ht="28" x14ac:dyDescent="0.2">
       <c r="A21" s="34" t="s">
-        <v>94</v>
+        <v>58</v>
       </c>
       <c r="B21" s="36">
         <v>0</v>
       </c>
       <c r="C21" s="22" t="s">
-        <v>95</v>
+        <v>80</v>
       </c>
       <c r="D21" s="35" t="s">
-        <v>96</v>
+        <v>60</v>
       </c>
       <c r="E21" s="36">
         <v>0</v>
       </c>
       <c r="F21" s="22" t="s">
-        <v>97</v>
+        <v>81</v>
       </c>
       <c r="G21" s="32"/>
       <c r="H21" s="19" t="s">
-        <v>98</v>
+        <v>82</v>
       </c>
       <c r="I21" s="14" t="s">
         <v>16</v>
@@ -2932,26 +2938,26 @@
     </row>
     <row r="22" spans="1:9" ht="36" x14ac:dyDescent="0.2">
       <c r="A22" s="37" t="s">
-        <v>99</v>
+        <v>43</v>
       </c>
       <c r="B22" s="36" t="s">
         <v>10</v>
       </c>
       <c r="C22" s="26" t="s">
-        <v>100</v>
+        <v>83</v>
       </c>
       <c r="D22" s="35" t="s">
-        <v>146</v>
+        <v>45</v>
       </c>
       <c r="E22" s="36">
         <v>0</v>
       </c>
       <c r="F22" s="26" t="s">
-        <v>102</v>
+        <v>84</v>
       </c>
       <c r="G22" s="32"/>
       <c r="H22" s="19" t="s">
-        <v>103</v>
+        <v>85</v>
       </c>
       <c r="I22" s="14" t="s">
         <v>16</v>
@@ -2959,26 +2965,26 @@
     </row>
     <row r="23" spans="1:9" ht="36" x14ac:dyDescent="0.2">
       <c r="A23" s="38" t="s">
-        <v>104</v>
+        <v>17</v>
       </c>
       <c r="B23" s="39" t="s">
         <v>13</v>
       </c>
       <c r="C23" s="31" t="s">
-        <v>105</v>
+        <v>86</v>
       </c>
       <c r="D23" s="40" t="s">
-        <v>44</v>
+        <v>19</v>
       </c>
       <c r="E23" s="39">
         <v>0</v>
       </c>
       <c r="F23" s="31" t="s">
-        <v>107</v>
+        <v>87</v>
       </c>
       <c r="G23" s="32"/>
       <c r="H23" s="19" t="s">
-        <v>108</v>
+        <v>88</v>
       </c>
       <c r="I23" s="14" t="s">
         <v>16</v>
@@ -2986,26 +2992,26 @@
     </row>
     <row r="24" spans="1:9" ht="28" x14ac:dyDescent="0.2">
       <c r="A24" s="34" t="s">
-        <v>109</v>
+        <v>187</v>
       </c>
       <c r="B24" s="36" t="s">
         <v>10</v>
       </c>
       <c r="C24" s="22" t="s">
-        <v>110</v>
+        <v>89</v>
       </c>
       <c r="D24" s="35" t="s">
-        <v>111</v>
+        <v>200</v>
       </c>
       <c r="E24" s="36">
         <v>0</v>
       </c>
       <c r="F24" s="22" t="s">
-        <v>112</v>
+        <v>90</v>
       </c>
       <c r="G24" s="12"/>
       <c r="H24" s="19" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="I24" s="14" t="s">
         <v>16</v>
@@ -3013,26 +3019,26 @@
     </row>
     <row r="25" spans="1:9" ht="28" x14ac:dyDescent="0.2">
       <c r="A25" s="37" t="s">
-        <v>113</v>
+        <v>21</v>
       </c>
       <c r="B25" s="36" t="s">
         <v>13</v>
       </c>
       <c r="C25" s="26" t="s">
-        <v>114</v>
+        <v>91</v>
       </c>
       <c r="D25" s="35" t="s">
-        <v>115</v>
+        <v>23</v>
       </c>
       <c r="E25" s="36" t="s">
         <v>13</v>
       </c>
       <c r="F25" s="26" t="s">
-        <v>116</v>
+        <v>92</v>
       </c>
       <c r="G25" s="12"/>
       <c r="H25" s="19" t="s">
-        <v>218</v>
+        <v>93</v>
       </c>
       <c r="I25" s="14" t="s">
         <v>16</v>
@@ -3040,327 +3046,327 @@
     </row>
     <row r="26" spans="1:9" ht="28" x14ac:dyDescent="0.2">
       <c r="A26" s="41" t="s">
-        <v>117</v>
+        <v>48</v>
       </c>
       <c r="B26" s="42">
         <v>0</v>
       </c>
       <c r="C26" s="42" t="s">
-        <v>118</v>
+        <v>95</v>
       </c>
       <c r="D26" s="43" t="s">
-        <v>119</v>
+        <v>50</v>
       </c>
       <c r="E26" s="42">
         <v>0</v>
       </c>
       <c r="F26" s="42" t="s">
-        <v>120</v>
+        <v>97</v>
       </c>
       <c r="G26" s="12"/>
       <c r="H26" s="44" t="s">
-        <v>208</v>
+        <v>98</v>
       </c>
       <c r="I26" s="14"/>
     </row>
-    <row r="27" spans="1:9" ht="169" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:9" ht="60" x14ac:dyDescent="0.2">
       <c r="A27" s="41" t="s">
-        <v>121</v>
+        <v>9</v>
       </c>
       <c r="B27" s="36">
         <v>0</v>
       </c>
       <c r="C27" s="42" t="s">
-        <v>122</v>
+        <v>100</v>
       </c>
       <c r="D27" s="43" t="s">
-        <v>63</v>
+        <v>12</v>
       </c>
       <c r="E27" s="42">
         <v>0</v>
       </c>
       <c r="F27" s="42" t="s">
-        <v>124</v>
+        <v>102</v>
       </c>
       <c r="G27" s="12"/>
       <c r="H27" s="44" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
       <c r="I27" s="22"/>
     </row>
     <row r="28" spans="1:9" ht="48" x14ac:dyDescent="0.2">
       <c r="A28" s="41" t="s">
-        <v>125</v>
+        <v>188</v>
       </c>
       <c r="B28" s="36">
         <v>0</v>
       </c>
       <c r="C28" s="42" t="s">
-        <v>126</v>
+        <v>104</v>
       </c>
       <c r="D28" s="43" t="s">
-        <v>29</v>
+        <v>201</v>
       </c>
       <c r="E28" s="42">
         <v>0</v>
       </c>
       <c r="F28" s="42" t="s">
-        <v>128</v>
+        <v>106</v>
       </c>
       <c r="H28" s="44" t="s">
-        <v>129</v>
+        <v>107</v>
       </c>
       <c r="I28" s="45"/>
     </row>
-    <row r="29" spans="1:9" ht="66" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:9" ht="36" x14ac:dyDescent="0.2">
       <c r="A29" s="41" t="s">
-        <v>130</v>
+        <v>189</v>
       </c>
       <c r="B29" s="22">
         <v>0</v>
       </c>
       <c r="C29" s="42" t="s">
-        <v>131</v>
+        <v>109</v>
       </c>
       <c r="D29" s="43" t="s">
-        <v>71</v>
+        <v>202</v>
       </c>
       <c r="E29" s="42">
         <v>0</v>
       </c>
       <c r="F29" s="42" t="s">
-        <v>133</v>
+        <v>111</v>
       </c>
       <c r="H29" s="19" t="s">
-        <v>214</v>
+        <v>112</v>
       </c>
       <c r="I29" s="45"/>
     </row>
     <row r="30" spans="1:9" ht="28" x14ac:dyDescent="0.2">
       <c r="A30" s="41" t="s">
-        <v>134</v>
+        <v>52</v>
       </c>
       <c r="B30" s="42" t="s">
         <v>13</v>
       </c>
       <c r="C30" s="42" t="s">
-        <v>135</v>
+        <v>114</v>
       </c>
       <c r="D30" s="43" t="s">
-        <v>49</v>
+        <v>54</v>
       </c>
       <c r="E30" s="22" t="s">
         <v>13</v>
       </c>
       <c r="F30" s="42" t="s">
-        <v>137</v>
+        <v>116</v>
       </c>
       <c r="H30" s="19" t="s">
-        <v>138</v>
+        <v>117</v>
       </c>
       <c r="I30" s="45"/>
     </row>
     <row r="31" spans="1:9" ht="36" x14ac:dyDescent="0.2">
       <c r="A31" s="46" t="s">
-        <v>139</v>
+        <v>31</v>
       </c>
       <c r="B31" s="42" t="s">
         <v>10</v>
       </c>
       <c r="C31" s="42" t="s">
-        <v>140</v>
+        <v>119</v>
       </c>
       <c r="D31" s="47" t="s">
-        <v>141</v>
+        <v>33</v>
       </c>
       <c r="E31" s="27" t="s">
         <v>13</v>
       </c>
       <c r="F31" s="22" t="s">
-        <v>142</v>
+        <v>121</v>
       </c>
       <c r="H31" s="19" t="s">
-        <v>143</v>
+        <v>122</v>
       </c>
       <c r="I31" s="45"/>
     </row>
     <row r="32" spans="1:9" ht="36" x14ac:dyDescent="0.2">
       <c r="A32" s="41" t="s">
-        <v>144</v>
+        <v>118</v>
       </c>
       <c r="B32" s="42">
         <v>0</v>
       </c>
       <c r="C32" s="42" t="s">
-        <v>145</v>
+        <v>124</v>
       </c>
       <c r="D32" s="43" t="s">
-        <v>101</v>
+        <v>120</v>
       </c>
       <c r="E32" s="22">
         <v>0</v>
       </c>
       <c r="F32" s="22" t="s">
-        <v>147</v>
+        <v>211</v>
       </c>
       <c r="H32" s="19" t="s">
-        <v>148</v>
+        <v>126</v>
       </c>
       <c r="I32" s="45"/>
     </row>
-    <row r="33" spans="1:9" ht="36" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:9" ht="48" x14ac:dyDescent="0.2">
       <c r="A33" s="48" t="s">
-        <v>149</v>
+        <v>63</v>
       </c>
       <c r="B33" s="42" t="s">
         <v>10</v>
       </c>
       <c r="C33" s="42" t="s">
-        <v>150</v>
+        <v>128</v>
       </c>
       <c r="D33" s="49" t="s">
-        <v>34</v>
+        <v>203</v>
       </c>
       <c r="E33" s="50" t="s">
         <v>10</v>
       </c>
       <c r="F33" s="50" t="s">
-        <v>152</v>
+        <v>129</v>
       </c>
       <c r="H33" s="51" t="s">
-        <v>209</v>
+        <v>130</v>
       </c>
       <c r="I33" s="45"/>
     </row>
     <row r="34" spans="1:9" ht="28" x14ac:dyDescent="0.2">
       <c r="A34" s="41" t="s">
-        <v>153</v>
+        <v>36</v>
       </c>
       <c r="B34" s="22" t="s">
         <v>10</v>
       </c>
       <c r="C34" s="42" t="s">
-        <v>154</v>
+        <v>132</v>
       </c>
       <c r="D34" s="43" t="s">
-        <v>24</v>
+        <v>38</v>
       </c>
       <c r="E34" s="22" t="s">
         <v>10</v>
       </c>
       <c r="F34" s="22" t="s">
-        <v>156</v>
+        <v>134</v>
       </c>
       <c r="H34" s="19" t="s">
-        <v>210</v>
+        <v>135</v>
       </c>
       <c r="I34" s="45"/>
     </row>
     <row r="35" spans="1:9" ht="28" x14ac:dyDescent="0.2">
       <c r="A35" s="52" t="s">
-        <v>157</v>
+        <v>65</v>
       </c>
       <c r="B35" s="42">
         <v>0</v>
       </c>
       <c r="C35" s="22" t="s">
-        <v>158</v>
+        <v>137</v>
       </c>
       <c r="D35" s="53" t="s">
-        <v>159</v>
+        <v>204</v>
       </c>
       <c r="E35" s="27" t="s">
         <v>10</v>
       </c>
       <c r="F35" s="22" t="s">
-        <v>160</v>
+        <v>138</v>
       </c>
       <c r="H35" s="19" t="s">
-        <v>161</v>
+        <v>139</v>
       </c>
       <c r="I35" s="45"/>
     </row>
     <row r="36" spans="1:9" ht="28" x14ac:dyDescent="0.2">
       <c r="A36" s="52" t="s">
-        <v>162</v>
+        <v>190</v>
       </c>
       <c r="B36" s="27" t="s">
         <v>13</v>
       </c>
       <c r="C36" s="22" t="s">
-        <v>163</v>
+        <v>141</v>
       </c>
       <c r="D36" s="53" t="s">
-        <v>54</v>
+        <v>205</v>
       </c>
       <c r="E36" s="27" t="s">
         <v>10</v>
       </c>
       <c r="F36" s="22" t="s">
-        <v>165</v>
+        <v>143</v>
       </c>
       <c r="H36" s="19" t="s">
-        <v>166</v>
+        <v>214</v>
       </c>
       <c r="I36" s="45"/>
     </row>
     <row r="37" spans="1:9" ht="29" x14ac:dyDescent="0.2">
       <c r="A37" s="52" t="s">
-        <v>167</v>
+        <v>191</v>
       </c>
       <c r="B37" s="27" t="s">
         <v>10</v>
       </c>
       <c r="C37" s="22" t="s">
-        <v>168</v>
+        <v>144</v>
       </c>
       <c r="D37" s="53" t="s">
-        <v>91</v>
+        <v>206</v>
       </c>
       <c r="E37" s="27">
         <v>0</v>
       </c>
       <c r="F37" s="54" t="s">
-        <v>170</v>
+        <v>213</v>
       </c>
       <c r="H37" s="19" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="I37" s="45"/>
     </row>
-    <row r="38" spans="1:9" ht="29" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:9" ht="48" x14ac:dyDescent="0.2">
       <c r="A38" s="52" t="s">
-        <v>171</v>
+        <v>192</v>
       </c>
       <c r="B38" s="27" t="s">
         <v>10</v>
       </c>
       <c r="C38" s="22" t="s">
-        <v>172</v>
+        <v>146</v>
       </c>
       <c r="D38" s="53" t="s">
-        <v>39</v>
+        <v>207</v>
       </c>
       <c r="E38" s="27" t="s">
         <v>10</v>
       </c>
       <c r="F38" s="54" t="s">
-        <v>174</v>
+        <v>212</v>
       </c>
       <c r="H38" s="19" t="s">
-        <v>211</v>
+        <v>148</v>
       </c>
       <c r="I38" s="45"/>
     </row>
     <row r="39" spans="1:9" ht="28" x14ac:dyDescent="0.2">
       <c r="A39" s="52" t="s">
-        <v>175</v>
+        <v>217</v>
       </c>
       <c r="B39" s="42" t="s">
         <v>10</v>
       </c>
       <c r="C39" s="22" t="s">
-        <v>176</v>
+        <v>150</v>
       </c>
       <c r="D39" s="55"/>
       <c r="E39" s="31"/>
@@ -3370,13 +3376,13 @@
     </row>
     <row r="40" spans="1:9" ht="28" x14ac:dyDescent="0.2">
       <c r="A40" s="41" t="s">
-        <v>177</v>
+        <v>27</v>
       </c>
       <c r="B40" s="22">
         <v>0</v>
       </c>
       <c r="C40" s="42" t="s">
-        <v>178</v>
+        <v>152</v>
       </c>
       <c r="D40" s="57"/>
       <c r="E40" s="45"/>
@@ -3403,10 +3409,10 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" s="58" t="s">
-        <v>179</v>
+        <v>153</v>
       </c>
       <c r="M1" s="58" t="s">
-        <v>180</v>
+        <v>154</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.2">
@@ -3415,33 +3421,33 @@
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" s="58" t="s">
-        <v>181</v>
+        <v>155</v>
       </c>
       <c r="M3" s="58" t="s">
-        <v>182</v>
+        <v>156</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" s="58"/>
       <c r="M4" s="58" t="s">
-        <v>183</v>
+        <v>157</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" s="58" t="s">
-        <v>184</v>
+        <v>158</v>
       </c>
       <c r="M5" s="58"/>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A6" s="58"/>
       <c r="M6" s="58" t="s">
-        <v>185</v>
+        <v>159</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A7" s="58" t="s">
-        <v>186</v>
+        <v>160</v>
       </c>
       <c r="M7" s="58"/>
     </row>
@@ -3451,26 +3457,26 @@
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A9" s="58" t="s">
-        <v>187</v>
+        <v>161</v>
       </c>
       <c r="M9" s="59" t="s">
-        <v>188</v>
+        <v>162</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A10" s="58" t="s">
-        <v>189</v>
+        <v>163</v>
       </c>
       <c r="M10" s="59" t="s">
-        <v>190</v>
+        <v>164</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A11" s="58" t="s">
-        <v>191</v>
+        <v>165</v>
       </c>
       <c r="M11" s="59" t="s">
-        <v>192</v>
+        <v>166</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.2">
@@ -3478,7 +3484,7 @@
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A13" s="58" t="s">
-        <v>193</v>
+        <v>167</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.2">
@@ -3486,7 +3492,7 @@
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A15" s="58" t="s">
-        <v>194</v>
+        <v>168</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.2">
@@ -3494,7 +3500,7 @@
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" s="58" t="s">
-        <v>195</v>
+        <v>169</v>
       </c>
     </row>
     <row r="18" spans="1:11" x14ac:dyDescent="0.2">
@@ -3502,65 +3508,65 @@
     </row>
     <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" s="59" t="s">
-        <v>188</v>
+        <v>162</v>
       </c>
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20" s="59" t="s">
-        <v>190</v>
+        <v>164</v>
       </c>
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21" s="59" t="s">
-        <v>192</v>
+        <v>166</v>
       </c>
     </row>
     <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24" s="59" t="s">
-        <v>196</v>
+        <v>170</v>
       </c>
     </row>
     <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25" s="59" t="s">
-        <v>197</v>
+        <v>171</v>
       </c>
       <c r="B25" t="s">
-        <v>198</v>
+        <v>172</v>
       </c>
       <c r="H25" t="s">
-        <v>199</v>
+        <v>173</v>
       </c>
     </row>
     <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A26" s="59" t="s">
-        <v>200</v>
+        <v>174</v>
       </c>
       <c r="B26" t="s">
-        <v>201</v>
+        <v>175</v>
       </c>
     </row>
     <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A27" s="59" t="s">
-        <v>202</v>
+        <v>176</v>
       </c>
       <c r="B27" t="s">
-        <v>203</v>
+        <v>177</v>
       </c>
       <c r="H27" t="s">
-        <v>204</v>
+        <v>178</v>
       </c>
       <c r="K27" t="s">
-        <v>205</v>
+        <v>179</v>
       </c>
     </row>
     <row r="29" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A29" s="59" t="s">
-        <v>206</v>
+        <v>180</v>
       </c>
     </row>
     <row r="30" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A30" s="59" t="s">
-        <v>207</v>
+        <v>181</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Remove redundant information from obfuscated excel
</commit_message>
<xml_diff>
--- a/tests/test_utilities/patient_data_2020_07_obfuscated.xlsx
+++ b/tests/test_utilities/patient_data_2020_07_obfuscated.xlsx
@@ -8,8 +8,7 @@
     <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="podklady pro Chromého" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="informail" sheetId="2" state="visible" r:id="rId3"/>
+    <sheet name="data" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -21,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="284" uniqueCount="219">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="252" uniqueCount="190">
   <si>
     <t xml:space="preserve">DONOR</t>
   </si>
@@ -180,7 +179,7 @@
     </r>
   </si>
   <si>
-    <t xml:space="preserve">Negativní</t>
+    <t xml:space="preserve">Negative</t>
   </si>
   <si>
     <t xml:space="preserve">128A-IND-D</t>
@@ -1543,124 +1542,6 @@
   </si>
   <si>
     <t xml:space="preserve">DQ9 DQ8 DP13 DR4 DQ4 DR51 DP14 DR7 DR13</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dobrý den, </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Dobrý den,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Posílám finální verzi tabulky.</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Teď přišla zpráva z Izraele – </t>
-    </r>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <u val="single"/>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">pár č. 1034</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve"> musíme vyškrtnout z párování!!</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">Víc informací nemám.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Česká skupina má v tomto párování bridging donora a altruistu. Určitě by bylo fajn uplatnění bridging (D12).</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Díky moc,</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Párovat se budou varianty:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CZ – WIEN varianty s možnostmi AB0i Tx (možnosti obě – jak kompatibilní Tx tak přes krevní skupinu)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Renata Zámečníková</t>
-  </si>
-  <si>
-    <t xml:space="preserve">CZ – IZRAEL pouze varianty AB0 kompatibilní transplantace </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Koordinátorka programu transplantací ledvin od žijících dárců</t>
-  </si>
-  <si>
-    <t xml:space="preserve">IZRAEL a WIEN se společně nepárují. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">+420 602 162 489</t>
-  </si>
-  <si>
-    <t xml:space="preserve">V případě potřeby jsem k dispozici na telefonu.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Pavlovi Chromému posílám stejné zadání.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">S pozdravem, </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Poznamky:</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cesi</t>
-  </si>
-  <si>
-    <t xml:space="preserve">prvni Idcka bez pocatecniho pismene (D1-D13)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">D12 bridge, D13 altruista</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Rakusaci</t>
-  </si>
-  <si>
-    <t xml:space="preserve">idcka zacinajici na W</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Israleci</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Posledni Idcka bez pocatecniho pismene(D1001-D1038)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">D1037 a D1038 altruista</t>
-  </si>
-  <si>
-    <t xml:space="preserve">D,R1034 vyrazen</t>
-  </si>
-  <si>
-    <t xml:space="preserve">U Rakusaku se predpoklada, ze ma akceptovatelne vsechny krevni skupiny (a budou to zrejme manualne upravovat)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">U Izraelcu jenom ty prirozene akceptovatelne - tedy ne AB0i protokol</t>
   </si>
 </sst>
 </file>
@@ -1670,7 +1551,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="19">
+  <fonts count="16">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1772,29 +1653,6 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <b val="true"/>
-      <u val="single"/>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF1F3864"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
-    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -1903,7 +1761,7 @@
       <protection locked="true" hidden="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="37">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2050,14 +1908,6 @@
     </xf>
     <xf numFmtId="164" fontId="15" fillId="0" borderId="1" xfId="24" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -2124,7 +1974,7 @@
       <rgbColor rgb="FFFF6600"/>
       <rgbColor rgb="FF666699"/>
       <rgbColor rgb="FF969696"/>
-      <rgbColor rgb="FF1F3864"/>
+      <rgbColor rgb="FF003366"/>
       <rgbColor rgb="FF339966"/>
       <rgbColor rgb="FF003300"/>
       <rgbColor rgb="FF333300"/>
@@ -2144,8 +1994,8 @@
   </sheetPr>
   <dimension ref="A2:I40"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F8" activeCellId="0" sqref="F8"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A25" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H37" activeCellId="0" sqref="H37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.515625" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2429,7 +2279,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="24.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="8" t="s">
         <v>57</v>
       </c>
@@ -2534,7 +2384,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="24.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="8" t="s">
         <v>78</v>
       </c>
@@ -3042,7 +2892,7 @@
       </c>
       <c r="I36" s="13"/>
     </row>
-    <row r="37" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" customFormat="false" ht="24.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="8" t="s">
         <v>174</v>
       </c>
@@ -3146,190 +2996,4 @@
     <oddFooter/>
   </headerFooter>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:M30"/>
-  <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A31" activeCellId="0" sqref="A31"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <sheetData>
-    <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="37" t="s">
-        <v>190</v>
-      </c>
-      <c r="M1" s="37" t="s">
-        <v>191</v>
-      </c>
-    </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="37"/>
-      <c r="M2" s="37"/>
-    </row>
-    <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="37" t="s">
-        <v>192</v>
-      </c>
-      <c r="M3" s="37" t="s">
-        <v>193</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="37"/>
-      <c r="M4" s="37" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="37" t="s">
-        <v>195</v>
-      </c>
-      <c r="M5" s="37"/>
-    </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="37"/>
-      <c r="M6" s="37" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="37" t="s">
-        <v>197</v>
-      </c>
-      <c r="M7" s="37"/>
-    </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="37"/>
-      <c r="M8" s="37"/>
-    </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="37" t="s">
-        <v>198</v>
-      </c>
-      <c r="M9" s="38" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="37" t="s">
-        <v>200</v>
-      </c>
-      <c r="M10" s="38" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="37" t="s">
-        <v>202</v>
-      </c>
-      <c r="M11" s="38" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="37"/>
-    </row>
-    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="37" t="s">
-        <v>204</v>
-      </c>
-    </row>
-    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="37"/>
-    </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="37" t="s">
-        <v>205</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="37"/>
-    </row>
-    <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="37" t="s">
-        <v>206</v>
-      </c>
-    </row>
-    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="37"/>
-    </row>
-    <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="38" t="s">
-        <v>199</v>
-      </c>
-    </row>
-    <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="38" t="s">
-        <v>201</v>
-      </c>
-    </row>
-    <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="38" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A24" s="38" t="s">
-        <v>207</v>
-      </c>
-    </row>
-    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="38" t="s">
-        <v>208</v>
-      </c>
-      <c r="B25" s="0" t="s">
-        <v>209</v>
-      </c>
-      <c r="H25" s="0" t="s">
-        <v>210</v>
-      </c>
-    </row>
-    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="38" t="s">
-        <v>211</v>
-      </c>
-      <c r="B26" s="0" t="s">
-        <v>212</v>
-      </c>
-    </row>
-    <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="38" t="s">
-        <v>213</v>
-      </c>
-      <c r="B27" s="0" t="s">
-        <v>214</v>
-      </c>
-      <c r="H27" s="0" t="s">
-        <v>215</v>
-      </c>
-      <c r="K27" s="0" t="s">
-        <v>216</v>
-      </c>
-    </row>
-    <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A29" s="38" t="s">
-        <v>217</v>
-      </c>
-    </row>
-    <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="38" t="s">
-        <v>218</v>
-      </c>
-    </row>
-  </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
-</worksheet>
 </file>
</xml_diff>